<commit_message>
bugfix in BOM (thanks to Sefirosu789 and unmaker from shmups forumfor pointing that out!)
</commit_message>
<xml_diff>
--- a/generalRGBmod/Main-PCB/v2/BOM_n64rgbv2.xlsx
+++ b/generalRGBmod/Main-PCB/v2/BOM_n64rgbv2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\Peter\Documents\Workspaces\Git\Mirror\n64rgb\generalRGBmod\Main-PCB\v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Peter\Documents\Workspaces\Git\Eigenes\n64rgb\generalRGBmod\Main-PCB\v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AED4F1-E691-4722-8A97-C928527E696C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FA9FA3-96EF-4008-B902-F2DE1428C868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="0" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MaxV Setup" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="114">
   <si>
     <t>Designator</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>BLM18PG471SN1D</t>
-  </si>
-  <si>
-    <t>GRM31CR61A476ME15L</t>
   </si>
   <si>
     <t>Ferrit bead</t>
@@ -401,6 +398,12 @@
   </si>
   <si>
     <t>Close J1, Alternative part: 5M570ZT100C4N</t>
+  </si>
+  <si>
+    <t>Value of MPN reference differs to ideal value to allow for negative margin!</t>
+  </si>
+  <si>
+    <t>GRM188R61E106KA73D</t>
   </si>
 </sst>
 </file>
@@ -1247,20 +1250,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="7" max="7" width="59.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1283,18 +1286,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1306,12 +1309,12 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -1322,55 +1325,55 @@
         <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
         <v>39</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>41</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" t="s">
         <v>81</v>
-      </c>
-      <c r="F7" t="s">
-        <v>82</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
@@ -1387,23 +1390,23 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1412,17 +1415,17 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -1431,7 +1434,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
@@ -1439,23 +1442,23 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -1464,20 +1467,20 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
         <v>46</v>
-      </c>
-      <c r="F15" t="s">
-        <v>47</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -1486,7 +1489,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" t="s">
         <v>11</v>
@@ -1494,12 +1497,12 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1508,7 +1511,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
@@ -1516,12 +1519,12 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1530,7 +1533,7 @@
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
         <v>25</v>
@@ -1538,12 +1541,12 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
         <v>55</v>
-      </c>
-      <c r="B19" t="s">
-        <v>56</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1552,7 +1555,7 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
@@ -1560,12 +1563,12 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
         <v>60</v>
-      </c>
-      <c r="B20" t="s">
-        <v>61</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1574,7 +1577,7 @@
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
         <v>11</v>
@@ -1582,15 +1585,728 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E25" s="2"/>
+      <c r="G25" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>76</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" t="s">
+        <v>108</v>
+      </c>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E45" s="2"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E47" s="2"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E49" s="2"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E50" s="2"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E51" s="2"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A38:B38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
@@ -1604,21 +2320,21 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F22" t="s">
         <v>11</v>
@@ -1626,12 +2342,12 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1639,46 +2355,32 @@
       <c r="D23" t="s">
         <v>12</v>
       </c>
-      <c r="E23" t="s">
-        <v>38</v>
+      <c r="E23" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="F23" t="s">
         <v>11</v>
       </c>
+      <c r="G23" t="s">
+        <v>74</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F24" t="s">
-        <v>11</v>
-      </c>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E24" s="2"/>
       <c r="G24" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -1687,7 +2389,7 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F25" t="s">
         <v>11</v>
@@ -1695,12 +2397,12 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1709,7 +2411,7 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F26" t="s">
         <v>11</v>
@@ -1717,12 +2419,12 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
         <v>69</v>
-      </c>
-      <c r="B27" t="s">
-        <v>70</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1731,7 +2433,7 @@
         <v>12</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F27" t="s">
         <v>11</v>
@@ -1739,65 +2441,65 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
       <c r="D28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="F30" t="s">
         <v>8</v>
@@ -1805,92 +2507,93 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E31" s="2"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>108</v>
-      </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C38">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F38" t="s">
         <v>8</v>
       </c>
       <c r="G38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>13</v>
       </c>
@@ -1903,55 +2606,55 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="2"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="2"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E48" s="2"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E49" s="2"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E50" s="2"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
     </row>
   </sheetData>
@@ -1962,688 +2665,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="7" max="7" width="59.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>97</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>99</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" t="s">
-        <v>82</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G8" s="3"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" t="s">
-        <v>75</v>
-      </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27" t="s">
-        <v>103</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F27" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>100</v>
-      </c>
-      <c r="D28" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" t="s">
-        <v>105</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E30" s="2"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="G31" t="s">
-        <v>77</v>
-      </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34" t="s">
-        <v>95</v>
-      </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="3"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>108</v>
-      </c>
-      <c r="B37" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F37" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" t="s">
-        <v>109</v>
-      </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E43" s="2"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E45" s="2"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E47" s="2"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E48" s="2"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E49" s="2"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B53" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A36:B36"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>